<commit_message>
adding intern projects domains
</commit_message>
<xml_diff>
--- a/src/test/resources/excelData.xlsx
+++ b/src/test/resources/excelData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ibrahim\IdeaProjects\webseit-test\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E65F701-6D2E-4A1D-8D72-AB0A3DF73A4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9F20126-C9F2-4C59-BE6D-153C5415BD73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12" yWindow="12" windowWidth="23016" windowHeight="12216" xr2:uid="{1A0E7E13-4B51-4D68-A319-BB2E1A6F5F75}"/>
+    <workbookView xWindow="2328" yWindow="144" windowWidth="20076" windowHeight="12096" xr2:uid="{1A0E7E13-4B51-4D68-A319-BB2E1A6F5F75}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="244">
   <si>
     <t>autoankauf-saarlouis.de</t>
   </si>
@@ -742,6 +742,30 @@
   </si>
   <si>
     <t>schrottunna.de</t>
+  </si>
+  <si>
+    <t>amjis.com</t>
+  </si>
+  <si>
+    <t>ilamecca.de</t>
+  </si>
+  <si>
+    <t>kalender.amjis.com</t>
+  </si>
+  <si>
+    <t>nivontec.de</t>
+  </si>
+  <si>
+    <t>nordstern.gmbh</t>
+  </si>
+  <si>
+    <t>nma-hamburg.de</t>
+  </si>
+  <si>
+    <t>smarttech-elektro.de</t>
+  </si>
+  <si>
+    <t>dr-elrafei.de</t>
   </si>
 </sst>
 </file>
@@ -764,7 +788,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -774,6 +798,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -799,7 +829,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -807,6 +837,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1121,10 +1152,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87EF5093-2B8D-4748-B826-5F7196BA71A3}">
-  <dimension ref="A1:B236"/>
+  <dimension ref="A1:B244"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A224" workbookViewId="0">
+      <selection activeCell="B244" sqref="B244"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2863,7 +2894,7 @@
     </row>
     <row r="193" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A193" t="str">
-        <f t="shared" ref="A193:A236" si="3">"https://www." &amp; B193</f>
+        <f t="shared" ref="A193:A243" si="3">"https://www." &amp; B193</f>
         <v>https://www.auto-ankauf-magdeburg.de</v>
       </c>
       <c r="B193" s="1" t="s">
@@ -3255,6 +3286,78 @@
       </c>
       <c r="B236" s="4" t="s">
         <v>235</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A237" t="str">
+        <f t="shared" si="3"/>
+        <v>https://www.amjis.com</v>
+      </c>
+      <c r="B237" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A238" t="str">
+        <f t="shared" si="3"/>
+        <v>https://www.ilamecca.de</v>
+      </c>
+      <c r="B238" s="5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A239" t="str">
+        <f t="shared" si="3"/>
+        <v>https://www.kalender.amjis.com</v>
+      </c>
+      <c r="B239" s="5" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A240" t="str">
+        <f t="shared" si="3"/>
+        <v>https://www.nivontec.de</v>
+      </c>
+      <c r="B240" s="5" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A241" t="str">
+        <f t="shared" si="3"/>
+        <v>https://www.nordstern.gmbh</v>
+      </c>
+      <c r="B241" s="5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A242" t="str">
+        <f t="shared" si="3"/>
+        <v>https://www.nma-hamburg.de</v>
+      </c>
+      <c r="B242" s="5" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A243" t="str">
+        <f t="shared" si="3"/>
+        <v>https://www.smarttech-elektro.de</v>
+      </c>
+      <c r="B243" s="5" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A244" t="str">
+        <f>"https://" &amp; B244</f>
+        <v>https://dr-elrafei.de</v>
+      </c>
+      <c r="B244" t="s">
+        <v>243</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating amjis to stonepulse
</commit_message>
<xml_diff>
--- a/src/test/resources/excelData.xlsx
+++ b/src/test/resources/excelData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ibrahim\IdeaProjects\webseit-test\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C16AACE-8731-4092-95BC-8BFBE6476F1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71943361-3102-4B8E-BF5C-1EDC6279891E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2328" yWindow="144" windowWidth="20076" windowHeight="12096" xr2:uid="{1A0E7E13-4B51-4D68-A319-BB2E1A6F5F75}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12240" xr2:uid="{1A0E7E13-4B51-4D68-A319-BB2E1A6F5F75}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="240">
   <si>
     <t>auto-ankauf-warendorf.de</t>
   </si>
@@ -726,9 +726,6 @@
     <t>amjis.com</t>
   </si>
   <si>
-    <t>kalender.amjis.com</t>
-  </si>
-  <si>
     <t>nivontec.de</t>
   </si>
   <si>
@@ -748,6 +745,15 @@
   </si>
   <si>
     <t>https://wiki.nordstern.gmbh/index.php?title=Hauptseite</t>
+  </si>
+  <si>
+    <t>key.stonepulse.de</t>
+  </si>
+  <si>
+    <t>todo.stonepulse.de</t>
+  </si>
+  <si>
+    <t>kalender.stonepulse.de</t>
   </si>
 </sst>
 </file>
@@ -1141,9 +1147,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87EF5093-2B8D-4748-B826-5F7196BA71A3}">
-  <dimension ref="A1:B246"/>
+  <dimension ref="A1:B241"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1162,2203 +1170,2158 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
-        <f>"https://www." &amp; B2</f>
-        <v>https://www.ilamecca.com</v>
+        <f t="shared" ref="A2:A4" si="0">"https://www." &amp; B2</f>
+        <v>https://www.key.stonepulse.de</v>
       </c>
       <c r="B2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
-        <f t="shared" ref="A3:A66" si="0">"https://www." &amp; B3</f>
-        <v>https://www.kalender.amjis.com</v>
+        <f t="shared" si="0"/>
+        <v>https://www.kalender.stonepulse.de</v>
       </c>
       <c r="B3" t="s">
-        <v>230</v>
+        <v>239</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
-        <v>https://www.nivontec.de</v>
+        <v>https://www.todo.stonepulse.de</v>
       </c>
       <c r="B4" t="s">
-        <v>231</v>
+        <v>238</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.nordstern.gmbh</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>232</v>
+        <f>"https://www." &amp; B5</f>
+        <v>https://www.ilamecca.com</v>
+      </c>
+      <c r="B5" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.nma-hamburg.de</v>
+        <f t="shared" ref="A6:A68" si="1">"https://www." &amp; B6</f>
+        <v>https://www.nivontec.de</v>
       </c>
       <c r="B6" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>237</v>
+      <c r="A7" t="str">
+        <f t="shared" si="1"/>
+        <v>https://www.nordstern.gmbh</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
+        <v>https://www.nma-hamburg.de</v>
+      </c>
+      <c r="B8" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="str">
+        <f t="shared" si="1"/>
         <v>https://www.smarttech-elektro.de</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B10" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="str">
+        <f>"https://" &amp; B11</f>
+        <v>https://dr-elrafei.de</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>234</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="str">
-        <f>"https://" &amp; B9</f>
-        <v>https://dr-elrafei.de</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.auto-ankauf-warendorf.de</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.autoankauf-flensburg.de</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.xn--auto-ankauf-osnabrck-6ec.de</v>
+        <f t="shared" si="1"/>
+        <v>https://www.auto-ankauf-warendorf.de</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.velbert-autoankauf.de</v>
+        <f t="shared" si="1"/>
+        <v>https://www.autoankauf-flensburg.de</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.recklinghausen-auto-ankauf.de</v>
+        <f t="shared" si="1"/>
+        <v>https://www.xn--auto-ankauf-osnabrck-6ec.de</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.autoankauf-rendsburg.de</v>
+        <f t="shared" si="1"/>
+        <v>https://www.velbert-autoankauf.de</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.autoankauf-kaiserslautern.de</v>
+        <f t="shared" si="1"/>
+        <v>https://www.recklinghausen-auto-ankauf.de</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.hamburg-auto-ankauf.de</v>
+        <f t="shared" si="1"/>
+        <v>https://www.autoankauf-rendsburg.de</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.mainz-auto.de</v>
+        <f t="shared" si="1"/>
+        <v>https://www.autoankauf-kaiserslautern.de</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.autoankauf-norderstedt.de</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>9</v>
+        <f t="shared" si="1"/>
+        <v>https://www.hamburg-auto-ankauf.de</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.bad-segeberg-autoankauf.de</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>10</v>
+        <f t="shared" si="1"/>
+        <v>https://www.mainz-auto.de</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.autoankauf-ahrensburg.de</v>
+        <f t="shared" si="1"/>
+        <v>https://www.autoankauf-norderstedt.de</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.xn--auto-ankauf-mnster-y6b.de</v>
+        <f t="shared" si="1"/>
+        <v>https://www.bad-segeberg-autoankauf.de</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.autowuppertal.de</v>
+        <f t="shared" si="1"/>
+        <v>https://www.autoankauf-ahrensburg.de</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.autoankauf-langenhagen.de</v>
+        <f t="shared" si="1"/>
+        <v>https://www.xn--auto-ankauf-mnster-y6b.de</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.xn--auto-ankauf-gtersloh-1ec.de</v>
+        <f t="shared" si="1"/>
+        <v>https://www.autowuppertal.de</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.auto-ankauf-giessen.de</v>
+        <f t="shared" si="1"/>
+        <v>https://www.autoankauf-langenhagen.de</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.xn--neumnster-auto-ankauf-cic.de</v>
+        <f t="shared" si="1"/>
+        <v>https://www.xn--auto-ankauf-gtersloh-1ec.de</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.bremen-auto-ankauf.de</v>
+        <f t="shared" si="1"/>
+        <v>https://www.auto-ankauf-giessen.de</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.wedel-autoankauf.de</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>19</v>
+        <f t="shared" si="1"/>
+        <v>https://www.xn--neumnster-auto-ankauf-cic.de</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.kfz-ankauf-hamm.de</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>20</v>
+        <f t="shared" si="1"/>
+        <v>https://www.bremen-auto-ankauf.de</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.auto-ankauf-fulda.de</v>
+        <f t="shared" si="1"/>
+        <v>https://www.wedel-autoankauf.de</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.xn--auto-ankauf-gttingen-gbc.de</v>
+        <f t="shared" si="1"/>
+        <v>https://www.kfz-ankauf-hamm.de</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.chemnitz-autoankauf.de</v>
+        <f t="shared" si="1"/>
+        <v>https://www.auto-ankauf-fulda.de</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.xn--auto-lneburg-ilb.de</v>
+        <f t="shared" si="1"/>
+        <v>https://www.xn--auto-ankauf-gttingen-gbc.de</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.auto-ankauf-euskirchen.de</v>
+        <f t="shared" si="1"/>
+        <v>https://www.chemnitz-autoankauf.de</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.rostock-autoankauf.de</v>
+        <f t="shared" si="1"/>
+        <v>https://www.xn--auto-lneburg-ilb.de</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.ingolstadt-auto-ankauf.de</v>
+        <f t="shared" si="1"/>
+        <v>https://www.auto-ankauf-euskirchen.de</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.xn--kln-auto-ankauf-8sb.de</v>
+        <f t="shared" si="1"/>
+        <v>https://www.rostock-autoankauf.de</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.xn--hxter-autoankauf-mwb.de</v>
+        <f t="shared" si="1"/>
+        <v>https://www.ingolstadt-auto-ankauf.de</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.kfz-ankauf-ulm.de</v>
+        <f t="shared" si="1"/>
+        <v>https://www.xn--kln-auto-ankauf-8sb.de</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.hildesheim-autoankauf.de</v>
+        <f t="shared" si="1"/>
+        <v>https://www.xn--hxter-autoankauf-mwb.de</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.kfz-ankauf-augsburg.de</v>
+        <f t="shared" si="1"/>
+        <v>https://www.kfz-ankauf-ulm.de</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.xn--auto-ankauf-lbeck-f3b.de</v>
+        <f t="shared" si="1"/>
+        <v>https://www.hildesheim-autoankauf.de</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.gummersbach-autoankauf.de</v>
+        <f t="shared" si="1"/>
+        <v>https://www.kfz-ankauf-augsburg.de</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.viersen-auto-ankauf.de</v>
+        <f t="shared" si="1"/>
+        <v>https://www.xn--auto-ankauf-lbeck-f3b.de</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.siegen-autoankauf.de</v>
+        <f t="shared" si="1"/>
+        <v>https://www.gummersbach-autoankauf.de</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.xn--auto-ankauf-saarbrcken-9lc.de</v>
+        <f t="shared" si="1"/>
+        <v>https://www.viersen-auto-ankauf.de</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.stade-autoankauf.de</v>
+        <f t="shared" si="1"/>
+        <v>https://www.siegen-autoankauf.de</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.autoankauf-diepholz.de</v>
+        <f t="shared" si="1"/>
+        <v>https://www.xn--auto-ankauf-saarbrcken-9lc.de</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A50" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.geesthacht-autoankauf.de</v>
+        <f t="shared" si="1"/>
+        <v>https://www.stade-autoankauf.de</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A51" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.auto-ankauf-dinslaken.de</v>
+        <f t="shared" si="1"/>
+        <v>https://www.autoankauf-diepholz.de</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.frankfurt-auto.de</v>
+        <f t="shared" si="1"/>
+        <v>https://www.geesthacht-autoankauf.de</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.xn--kfz-ankauf-dsseldorf-0ec.de</v>
+        <f t="shared" si="1"/>
+        <v>https://www.auto-ankauf-dinslaken.de</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A54" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.kfz-ankauf-hamburg.de</v>
+        <f t="shared" si="1"/>
+        <v>https://www.frankfurt-auto.de</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A55" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.berlin-auto-ankauf.de</v>
+        <f t="shared" si="1"/>
+        <v>https://www.xn--kfz-ankauf-dsseldorf-0ec.de</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A56" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.autoankauf-butzbach.de</v>
+        <f t="shared" si="1"/>
+        <v>https://www.kfz-ankauf-hamburg.de</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A57" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.autoankauf-bretten.de</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>47</v>
+        <f t="shared" si="1"/>
+        <v>https://www.berlin-auto-ankauf.de</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A58" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.xn--autoankauf-ldenscheid-kic.de</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>48</v>
+        <f t="shared" si="1"/>
+        <v>https://www.autoankauf-butzbach.de</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A59" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.autoankauf-aurich.de</v>
+        <f t="shared" si="1"/>
+        <v>https://www.autoankauf-bretten.de</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A60" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.autoankauf-cloppenburg.de</v>
+        <f t="shared" si="1"/>
+        <v>https://www.xn--autoankauf-ldenscheid-kic.de</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A61" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.auto-ankauf-aschaffenburg.de</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>51</v>
+        <f t="shared" si="1"/>
+        <v>https://www.autoankauf-aurich.de</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A62" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.autoankauf-baden-baden.de</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>52</v>
+        <f t="shared" si="1"/>
+        <v>https://www.autoankauf-cloppenburg.de</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A63" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.auto-ankauf-coesfeld.de</v>
+        <f t="shared" si="1"/>
+        <v>https://www.auto-ankauf-aschaffenburg.de</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A64" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.autoankauf-bad-hersfeld.de</v>
+        <f t="shared" si="1"/>
+        <v>https://www.autoankauf-baden-baden.de</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A65" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.braunschweig-auto-ankauf.de</v>
+        <f t="shared" si="1"/>
+        <v>https://www.auto-ankauf-coesfeld.de</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A66" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.freiberg-auto-ankauf.de</v>
+        <f t="shared" si="1"/>
+        <v>https://www.autoankauf-bad-hersfeld.de</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A67" t="str">
-        <f t="shared" ref="A67:A130" si="1">"https://www." &amp; B67</f>
-        <v>https://www.kfz-ankauf-fulda.de</v>
+        <f t="shared" si="1"/>
+        <v>https://www.braunschweig-auto-ankauf.de</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A68" t="str">
         <f t="shared" si="1"/>
-        <v>https://www.kfz-ankauf-eisenach.de</v>
+        <v>https://www.freiberg-auto-ankauf.de</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A69" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.auto-ankauf-darmstadt.de</v>
+        <f t="shared" ref="A69:A132" si="2">"https://www." &amp; B69</f>
+        <v>https://www.kfz-ankauf-fulda.de</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A70" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.dormagen-autoankauf.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.kfz-ankauf-eisenach.de</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A71" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.auto-ankauf-geldern.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.auto-ankauf-darmstadt.de</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A72" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.auto-ankauf-dachau.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.dormagen-autoankauf.de</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A73" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.erkrath-autoankauf.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.auto-ankauf-geldern.de</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A74" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.erfurt-autoankauf.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.auto-ankauf-dachau.de</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A75" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.autoankauf-steinborn.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.erkrath-autoankauf.de</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A76" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.autoankauf-meisburg.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.erfurt-autoankauf.de</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A77" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.autoankauf-birresborn.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.autoankauf-steinborn.de</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A78" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.autoankauf-odelzhausen.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.autoankauf-meisburg.de</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A79" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.autoankauf-cochem.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.autoankauf-birresborn.de</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A80" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.autoankauf-burghaun.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.autoankauf-odelzhausen.de</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A81" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.autoankauf-siegsdorf.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.autoankauf-cochem.de</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A82" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.autoankauf-pfarrkirchen.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.autoankauf-burghaun.de</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A83" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.autoankauf-hildburghausen.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.autoankauf-siegsdorf.de</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A84" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.autoankauf-weilburg.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.autoankauf-pfarrkirchen.de</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A85" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.autoankauf-finthen.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.autoankauf-hildburghausen.de</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A86" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.autoankauf-schwalmstadt.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.autoankauf-weilburg.de</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A87" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.autoankauf-warburg.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.autoankauf-finthen.de</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A88" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.autoankauf-sangerhausen.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.autoankauf-schwalmstadt.de</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A89" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.autoankauf-stendal.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.autoankauf-warburg.de</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A90" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.autoankauf-bad-salzungen.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.autoankauf-sangerhausen.de</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A91" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.autoankauf-steinburg.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.autoankauf-stendal.de</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A92" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.autoankauf-ratzeburg.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.autoankauf-bad-salzungen.de</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A93" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.autoankauf-mainburg.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.autoankauf-steinburg.de</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A94" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.autoankauf-bad-wildungen.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.autoankauf-ratzeburg.de</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A95" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.auto-ankauf-ravensburg.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.autoankauf-mainburg.de</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A96" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.autoankauf-preetz.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.autoankauf-bad-wildungen.de</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A97" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.autoankauf-wittlich.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.auto-ankauf-ravensburg.de</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A98" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.auto-ankauf-steinfurt.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.autoankauf-preetz.de</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A99" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.autoankauf-wittmund.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.autoankauf-wittlich.de</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A100" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.autoankauf-hungen.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.auto-ankauf-steinfurt.de</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A101" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.autoankauf-karlsbad.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.autoankauf-wittmund.de</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A102" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.autoankauf-brilon.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.autoankauf-hungen.de</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A103" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.autoankauf-homberg.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.autoankauf-karlsbad.de</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A104" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.herrenberg-autoankauf.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.autoankauf-brilon.de</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A105" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.autoankauf-pfaffenhofen.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.autoankauf-homberg.de</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A106" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.auto-ankauf-miltenberg.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.herrenberg-autoankauf.de</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A107" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.auto-ankauf-passau.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.autoankauf-pfaffenhofen.de</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A108" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.autoankauf-fritzlar.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.auto-ankauf-miltenberg.de</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A109" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.autoankauf-uelzen.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.auto-ankauf-passau.de</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A110" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.autoankauf-bad-kissingen.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.autoankauf-fritzlar.de</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A111" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.auto-ankauf-meppen.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.autoankauf-uelzen.de</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A112" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.unna-auto-ankauf.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.autoankauf-bad-kissingen.de</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A113" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.autoankauf-schwabach.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.auto-ankauf-meppen.de</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A114" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.autoankauf-emsland.de</v>
-      </c>
-      <c r="B114" s="3" t="s">
-        <v>104</v>
+        <f t="shared" si="2"/>
+        <v>https://www.unna-auto-ankauf.de</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A115" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.kleve-auto-ankauf.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.autoankauf-schwabach.de</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A116" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.autoankauf-dietzenbach.de</v>
-      </c>
-      <c r="B116" s="1" t="s">
-        <v>106</v>
+        <f t="shared" si="2"/>
+        <v>https://www.autoankauf-emsland.de</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A117" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.autoankauf-wernigerode.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.kleve-auto-ankauf.de</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A118" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.autoankauf-peine.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.autoankauf-dietzenbach.de</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A119" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.kfz-ankauf-mainz.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.autoankauf-wernigerode.de</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A120" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.autoankauf-merzig.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.autoankauf-peine.de</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A121" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.mayen-autoankauf.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.kfz-ankauf-mainz.de</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A122" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.oldenburg-auto-ankauf.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.autoankauf-merzig.de</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A123" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.kfz-ankauf-trier.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.mayen-autoankauf.de</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A124" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.auto-ankauf-daun.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.oldenburg-auto-ankauf.de</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A125" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.autoankauf-osterholz-scharmbeck.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.kfz-ankauf-trier.de</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A126" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.autoankauf-schwerin.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.auto-ankauf-daun.de</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A127" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.autoankauf-helmstedt.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.autoankauf-osterholz-scharmbeck.de</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A128" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.kfz-ankauf-marburg.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.autoankauf-schwerin.de</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A129" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.auto-ankauf-forchheim.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.autoankauf-helmstedt.de</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A130" t="str">
-        <f t="shared" si="1"/>
-        <v>https://www.auto-ankauf-ahaus.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.kfz-ankauf-marburg.de</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A131" t="str">
-        <f t="shared" ref="A131:A194" si="2">"https://www." &amp; B131</f>
-        <v>https://www.autoankauf-griesheim.de</v>
+        <f t="shared" si="2"/>
+        <v>https://www.auto-ankauf-forchheim.de</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A132" t="str">
         <f t="shared" si="2"/>
-        <v>https://www.autoankauf-sinsheim.de</v>
+        <v>https://www.auto-ankauf-ahaus.de</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A133" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.autoankauf-northeim.de</v>
+        <f t="shared" ref="A133:A196" si="3">"https://www." &amp; B133</f>
+        <v>https://www.autoankauf-griesheim.de</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A134" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.autoankauf-altenburg.de</v>
+        <f t="shared" si="3"/>
+        <v>https://www.autoankauf-sinsheim.de</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A135" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.autoankauf-murnau.de</v>
+        <f t="shared" si="3"/>
+        <v>https://www.autoankauf-northeim.de</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A136" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.salzgitter-autoankauf.de</v>
+        <f t="shared" si="3"/>
+        <v>https://www.autoankauf-altenburg.de</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A137" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.autoankauf-bautzen.de</v>
+        <f t="shared" si="3"/>
+        <v>https://www.autoankauf-murnau.de</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A138" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.autoankauf-konstanz.de</v>
+        <f t="shared" si="3"/>
+        <v>https://www.salzgitter-autoankauf.de</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A139" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.autoankauf-mosbach.de</v>
+        <f t="shared" si="3"/>
+        <v>https://www.autoankauf-bautzen.de</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A140" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.auto-ankauf-eppingen.de</v>
+        <f t="shared" si="3"/>
+        <v>https://www.autoankauf-konstanz.de</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A141" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.autoankauf-duderstadt.de</v>
+        <f t="shared" si="3"/>
+        <v>https://www.autoankauf-mosbach.de</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A142" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.autoankauf-bad-segeberg.de</v>
+        <f t="shared" si="3"/>
+        <v>https://www.auto-ankauf-eppingen.de</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A143" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.autohilden.de</v>
+        <f t="shared" si="3"/>
+        <v>https://www.autoankauf-duderstadt.de</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A144" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.autoankauf-gerolstein.de</v>
+        <f t="shared" si="3"/>
+        <v>https://www.autoankauf-bad-segeberg.de</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A145" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.auto-ankauf-butzbach.de</v>
+        <f t="shared" si="3"/>
+        <v>https://www.autohilden.de</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A146" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.auto-ankauf-pinneberg.de</v>
+        <f t="shared" si="3"/>
+        <v>https://www.autoankauf-gerolstein.de</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A147" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.autoankauf-offenburg.de</v>
+        <f t="shared" si="3"/>
+        <v>https://www.auto-ankauf-butzbach.de</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A148" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.autohaan.de</v>
+        <f t="shared" si="3"/>
+        <v>https://www.auto-ankauf-pinneberg.de</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A149" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.auto-ankauf-landshut.de</v>
+        <f t="shared" si="3"/>
+        <v>https://www.autoankauf-offenburg.de</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A150" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.autoankauf-bad-oldesloe.de</v>
+        <f t="shared" si="3"/>
+        <v>https://www.autohaan.de</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A151" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.auto-ankauf-bielefeld.de</v>
+        <f t="shared" si="3"/>
+        <v>https://www.auto-ankauf-landshut.de</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A152" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.kfz-ankauf-kiel.de</v>
+        <f t="shared" si="3"/>
+        <v>https://www.autoankauf-bad-oldesloe.de</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A153" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.autoankauf-gifhorn.de</v>
+        <f t="shared" si="3"/>
+        <v>https://www.auto-ankauf-bielefeld.de</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A154" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.autoankauf-pforzheim.de</v>
+        <f t="shared" si="3"/>
+        <v>https://www.kfz-ankauf-kiel.de</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A155" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.auto-ankauf-altenkirchen.de</v>
+        <f t="shared" si="3"/>
+        <v>https://www.autoankauf-gifhorn.de</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="156" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A156" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.auto-ankauf-neuwied.de</v>
+        <f t="shared" si="3"/>
+        <v>https://www.autoankauf-pforzheim.de</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A157" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.autoankauf-bad-nauheim.de</v>
+        <f t="shared" si="3"/>
+        <v>https://www.auto-ankauf-altenkirchen.de</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="158" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A158" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.auto-ankauf-memmingen.de</v>
+        <f t="shared" si="3"/>
+        <v>https://www.auto-ankauf-neuwied.de</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A159" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.wolfsburg-autoankauf.de</v>
+        <f t="shared" si="3"/>
+        <v>https://www.autoankauf-bad-nauheim.de</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A160" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.wermelskirchen-autoankauf.de</v>
+        <f t="shared" si="3"/>
+        <v>https://www.auto-ankauf-memmingen.de</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="161" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A161" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.auto-ankauf-traunstein.de</v>
+        <f t="shared" si="3"/>
+        <v>https://www.wolfsburg-autoankauf.de</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="162" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A162" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.kfz-ankauf-neubrandenburg.de</v>
+        <f t="shared" si="3"/>
+        <v>https://www.wermelskirchen-autoankauf.de</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A163" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.autoankauf-speyer.de</v>
+        <f t="shared" si="3"/>
+        <v>https://www.auto-ankauf-traunstein.de</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A164" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.auto-ankauf-witten.de</v>
-      </c>
-      <c r="B164" s="3" t="s">
-        <v>154</v>
+        <f t="shared" si="3"/>
+        <v>https://www.kfz-ankauf-neubrandenburg.de</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A165" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.leipzig-autoankauf.de</v>
+        <f t="shared" si="3"/>
+        <v>https://www.autoankauf-speyer.de</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A166" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.auto-ankauf-siegburg.de</v>
-      </c>
-      <c r="B166" s="1" t="s">
-        <v>156</v>
+        <f t="shared" si="3"/>
+        <v>https://www.auto-ankauf-witten.de</v>
+      </c>
+      <c r="B166" s="3" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A167" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.xn--autoankauf-tbingen-x6b.de</v>
+        <f t="shared" si="3"/>
+        <v>https://www.leipzig-autoankauf.de</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A168" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.kfz-ankauf-regensburg.de</v>
+        <f t="shared" si="3"/>
+        <v>https://www.auto-ankauf-siegburg.de</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="169" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A169" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.auto-ankauf-deggendorf.de</v>
+        <f t="shared" si="3"/>
+        <v>https://www.xn--autoankauf-tbingen-x6b.de</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A170" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.auto-ankauf-straubing.de</v>
+        <f t="shared" si="3"/>
+        <v>https://www.kfz-ankauf-regensburg.de</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A171" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.auto-ankauf-konstanz.de</v>
+        <f t="shared" si="3"/>
+        <v>https://www.auto-ankauf-deggendorf.de</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A172" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.auto-ankauf-ludwigsburg.de</v>
+        <f t="shared" si="3"/>
+        <v>https://www.auto-ankauf-straubing.de</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="173" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A173" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.auto-ankauf-rheine.de</v>
+        <f t="shared" si="3"/>
+        <v>https://www.auto-ankauf-konstanz.de</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A174" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.autoankauf-itzehoe.de</v>
+        <f t="shared" si="3"/>
+        <v>https://www.auto-ankauf-ludwigsburg.de</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="175" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A175" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.auto-ankauf-aalen.de</v>
+        <f t="shared" si="3"/>
+        <v>https://www.auto-ankauf-rheine.de</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A176" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.auto-ankauf-kempen.de</v>
+        <f t="shared" si="3"/>
+        <v>https://www.autoankauf-itzehoe.de</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A177" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.autoankauf-halle-saale.de</v>
+        <f t="shared" si="3"/>
+        <v>https://www.auto-ankauf-aalen.de</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A178" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.kfz-ankauf-nettetal.de</v>
+        <f t="shared" si="3"/>
+        <v>https://www.auto-ankauf-kempen.de</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A179" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.castrop-rauxel-autoankauf.de</v>
+        <f t="shared" si="3"/>
+        <v>https://www.autoankauf-halle-saale.de</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A180" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.xn--saarbrcken-gebrauchtwagenankauf-tid.de</v>
+        <f t="shared" si="3"/>
+        <v>https://www.kfz-ankauf-nettetal.de</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A181" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.auto-ankauf-lippstadt.de</v>
+        <f t="shared" si="3"/>
+        <v>https://www.castrop-rauxel-autoankauf.de</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A182" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.auto-ankauf-heinsberg.de</v>
+        <f t="shared" si="3"/>
+        <v>https://www.xn--saarbrcken-gebrauchtwagenankauf-tid.de</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A183" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.auto-ankauf-soest.de</v>
+        <f t="shared" si="3"/>
+        <v>https://www.auto-ankauf-lippstadt.de</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A184" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.auto-ankauf-amberg.de</v>
+        <f t="shared" si="3"/>
+        <v>https://www.auto-ankauf-heinsberg.de</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A185" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.halle-auto-ankauf.de</v>
+        <f t="shared" si="3"/>
+        <v>https://www.auto-ankauf-soest.de</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A186" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.autoankauf-dillenburg.de</v>
-      </c>
-      <c r="B186" s="3" t="s">
-        <v>176</v>
+        <f t="shared" si="3"/>
+        <v>https://www.auto-ankauf-amberg.de</v>
+      </c>
+      <c r="B186" s="1" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="187" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A187" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.schweinfurt-auto-ankauf.de</v>
+        <f t="shared" si="3"/>
+        <v>https://www.halle-auto-ankauf.de</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="188" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A188" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.kfz-ankauf-bielefeld.de</v>
-      </c>
-      <c r="B188" s="1" t="s">
-        <v>178</v>
+        <f t="shared" si="3"/>
+        <v>https://www.autoankauf-dillenburg.de</v>
+      </c>
+      <c r="B188" s="3" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="189" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A189" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.auto-ankauf-bamberg.de</v>
+        <f t="shared" si="3"/>
+        <v>https://www.schweinfurt-auto-ankauf.de</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="190" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A190" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.freiburg-auto-ankauf.de</v>
+        <f t="shared" si="3"/>
+        <v>https://www.kfz-ankauf-bielefeld.de</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="191" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A191" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.autoankauf-zwickau.de</v>
+        <f t="shared" si="3"/>
+        <v>https://www.auto-ankauf-bamberg.de</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="192" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A192" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.autoankauf-schleswig.de</v>
+        <f t="shared" si="3"/>
+        <v>https://www.freiburg-auto-ankauf.de</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="193" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A193" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.auto-ankauf-minden.de</v>
+        <f t="shared" si="3"/>
+        <v>https://www.autoankauf-zwickau.de</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="194" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A194" t="str">
-        <f t="shared" si="2"/>
-        <v>https://www.solingen-auto.de</v>
+        <f t="shared" si="3"/>
+        <v>https://www.autoankauf-schleswig.de</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="195" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A195" t="str">
-        <f t="shared" ref="A195:A245" si="3">"https://www." &amp; B195</f>
-        <v>https://www.auto-ankauf-magdeburg.de</v>
+        <f t="shared" si="3"/>
+        <v>https://www.auto-ankauf-minden.de</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="196" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A196" t="str">
         <f t="shared" si="3"/>
-        <v>https://www.gebrauchtwagen-ankauf-heilbronn.de</v>
+        <v>https://www.solingen-auto.de</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="197" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A197" t="str">
-        <f t="shared" si="3"/>
-        <v>https://www.xn--kfz-ankauf-wrzburg-x6b.de</v>
+        <f t="shared" ref="A197:A241" si="4">"https://www." &amp; B197</f>
+        <v>https://www.auto-ankauf-magdeburg.de</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="198" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A198" t="str">
-        <f t="shared" si="3"/>
-        <v>https://www.frankfurt-am-main-autoankauf.de</v>
+        <f t="shared" si="4"/>
+        <v>https://www.gebrauchtwagen-ankauf-heilbronn.de</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="199" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A199" t="str">
-        <f t="shared" si="3"/>
-        <v>https://www.xn--kfz-ankauf-mnster-e3b.de</v>
+        <f t="shared" si="4"/>
+        <v>https://www.xn--kfz-ankauf-wrzburg-x6b.de</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="200" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A200" t="str">
-        <f t="shared" si="3"/>
-        <v>https://www.auto-ankauf-krefeld24.de</v>
+        <f t="shared" si="4"/>
+        <v>https://www.frankfurt-am-main-autoankauf.de</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="201" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A201" t="str">
-        <f t="shared" si="3"/>
-        <v>https://www.gebrauchtwagen-ankauf-hannover.de</v>
+        <f t="shared" si="4"/>
+        <v>https://www.xn--kfz-ankauf-mnster-e3b.de</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="202" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A202" t="str">
-        <f t="shared" si="3"/>
-        <v>https://www.autoratingen.de</v>
+        <f t="shared" si="4"/>
+        <v>https://www.auto-ankauf-krefeld24.de</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="203" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A203" t="str">
-        <f t="shared" si="3"/>
-        <v>https://www.auto-ankauf-karlsruhe.de</v>
+        <f t="shared" si="4"/>
+        <v>https://www.gebrauchtwagen-ankauf-hannover.de</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="204" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A204" t="str">
-        <f t="shared" si="3"/>
-        <v>https://www.auto-ankauf-wesel.de</v>
+        <f t="shared" si="4"/>
+        <v>https://www.autoratingen.de</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A205" t="str">
-        <f t="shared" si="3"/>
-        <v>https://www.xn--kfz-ankauf-nrnberg-x6b.de</v>
+        <f t="shared" si="4"/>
+        <v>https://www.auto-ankauf-karlsruhe.de</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="206" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A206" t="str">
-        <f t="shared" si="3"/>
-        <v>https://www.kfz-ankauf-dresden.de</v>
+        <f t="shared" si="4"/>
+        <v>https://www.auto-ankauf-wesel.de</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="207" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A207" t="str">
-        <f t="shared" si="3"/>
-        <v>https://www.gebrauchtwagen-ankauf-mainz.de</v>
+        <f t="shared" si="4"/>
+        <v>https://www.xn--kfz-ankauf-nrnberg-x6b.de</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="208" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A208" t="str">
-        <f t="shared" si="3"/>
-        <v>https://www.kfz-ankauf-herne.de</v>
+        <f t="shared" si="4"/>
+        <v>https://www.kfz-ankauf-dresden.de</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="209" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A209" t="str">
-        <f t="shared" si="3"/>
-        <v>https://www.autoleverkusen.de</v>
+        <f t="shared" si="4"/>
+        <v>https://www.gebrauchtwagen-ankauf-mainz.de</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="210" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A210" t="str">
-        <f t="shared" si="3"/>
-        <v>https://www.kfz-ankauf-bochum.de</v>
+        <f t="shared" si="4"/>
+        <v>https://www.kfz-ankauf-herne.de</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="211" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A211" t="str">
-        <f t="shared" si="3"/>
-        <v>https://www.gebrauchtwagen-ankauf-ulm.de</v>
+        <f t="shared" si="4"/>
+        <v>https://www.autoleverkusen.de</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="212" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A212" t="str">
-        <f t="shared" si="3"/>
-        <v>https://www.xn--mnchen-auto-ankauf-m6b.de</v>
+        <f t="shared" si="4"/>
+        <v>https://www.kfz-ankauf-bochum.de</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="213" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A213" t="str">
-        <f t="shared" si="3"/>
-        <v>https://www.auto-ankauf-gelsenkirchen24.de</v>
+        <f t="shared" si="4"/>
+        <v>https://www.gebrauchtwagen-ankauf-ulm.de</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="214" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A214" t="str">
-        <f t="shared" si="3"/>
-        <v>https://www.gebrauchtwagen-ankauf-kassel.de</v>
+        <f t="shared" si="4"/>
+        <v>https://www.xn--mnchen-auto-ankauf-m6b.de</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="215" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A215" t="str">
-        <f t="shared" si="3"/>
-        <v>https://www.wiesbaden-auto-ankauf.de</v>
+        <f t="shared" si="4"/>
+        <v>https://www.auto-ankauf-gelsenkirchen24.de</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="216" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A216" t="str">
-        <f t="shared" si="3"/>
-        <v>https://www.xn--mnster-auto-ankauf-m6b.de</v>
+        <f t="shared" si="4"/>
+        <v>https://www.gebrauchtwagen-ankauf-kassel.de</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A217" t="str">
-        <f t="shared" si="3"/>
-        <v>https://www.autobonn.de</v>
+        <f t="shared" si="4"/>
+        <v>https://www.wiesbaden-auto-ankauf.de</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A218" t="str">
-        <f t="shared" si="3"/>
-        <v>https://www.gebrauchtwagen-ankauf-paderborn.de</v>
+        <f t="shared" si="4"/>
+        <v>https://www.xn--mnster-auto-ankauf-m6b.de</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A219" t="str">
-        <f t="shared" si="3"/>
-        <v>https://www.stuttgart-auto-ankauf.de</v>
+        <f t="shared" si="4"/>
+        <v>https://www.autobonn.de</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="220" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A220" t="str">
-        <f t="shared" si="3"/>
-        <v>https://www.kfz-ankauf-reutlingen.de</v>
+        <f t="shared" si="4"/>
+        <v>https://www.gebrauchtwagen-ankauf-paderborn.de</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A221" t="str">
-        <f t="shared" si="3"/>
-        <v>https://www.xn--autoankauf-gppingen-16b.de</v>
+        <f t="shared" si="4"/>
+        <v>https://www.stuttgart-auto-ankauf.de</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="222" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A222" t="str">
-        <f t="shared" si="3"/>
-        <v>https://www.gebrauchtwagen-ankauf-stuttgart.de</v>
+        <f t="shared" si="4"/>
+        <v>https://www.kfz-ankauf-reutlingen.de</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="223" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A223" t="str">
-        <f t="shared" si="3"/>
-        <v>https://www.autoduisburg.de</v>
+        <f t="shared" si="4"/>
+        <v>https://www.xn--autoankauf-gppingen-16b.de</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="224" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A224" t="str">
-        <f t="shared" si="3"/>
-        <v>https://www.auto-ankauf-herford.de</v>
+        <f t="shared" si="4"/>
+        <v>https://www.gebrauchtwagen-ankauf-stuttgart.de</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="225" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A225" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
+        <v>https://www.autoduisburg.de</v>
+      </c>
+      <c r="B225" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A226" t="str">
+        <f t="shared" si="4"/>
+        <v>https://www.auto-ankauf-herford.de</v>
+      </c>
+      <c r="B226" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A227" t="str">
+        <f t="shared" si="4"/>
         <v>https://www.dortmund-auto-ankauf.de</v>
       </c>
-      <c r="B225" s="1" t="s">
+      <c r="B227" s="1" t="s">
         <v>215</v>
-      </c>
-    </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A226" t="str">
-        <f t="shared" si="3"/>
-        <v>https://www.leverkusen-schrott.de</v>
-      </c>
-      <c r="B226" s="4" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A227" t="str">
-        <f t="shared" si="3"/>
-        <v>https://www.schrott-ankauf-bonn.de</v>
-      </c>
-      <c r="B227" s="4" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A228" t="str">
-        <f t="shared" si="3"/>
-        <v>https://www.schrott-ankauf-duisburg.de</v>
+        <f t="shared" si="4"/>
+        <v>https://www.leverkusen-schrott.de</v>
       </c>
       <c r="B228" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A229" t="str">
-        <f t="shared" si="3"/>
-        <v>https://www.schrott-ankauf-essen.de</v>
+        <f t="shared" si="4"/>
+        <v>https://www.schrott-ankauf-bonn.de</v>
       </c>
       <c r="B229" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A230" t="str">
-        <f t="shared" si="3"/>
-        <v>https://www.schrott-ankauf-gelsenkirchen.de</v>
+        <f t="shared" si="4"/>
+        <v>https://www.schrott-ankauf-duisburg.de</v>
       </c>
       <c r="B230" s="4" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A231" t="str">
-        <f t="shared" si="3"/>
-        <v>https://www.schrott-ankauf-wuppertal.de</v>
+        <f t="shared" si="4"/>
+        <v>https://www.schrott-ankauf-essen.de</v>
       </c>
       <c r="B231" s="4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A232" t="str">
-        <f t="shared" si="3"/>
-        <v>https://www.schrott-recklinghausen.de</v>
+        <f t="shared" si="4"/>
+        <v>https://www.schrott-ankauf-gelsenkirchen.de</v>
       </c>
       <c r="B232" s="4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A233" t="str">
-        <f t="shared" si="3"/>
-        <v>https://www.schrottgummersbach.de</v>
+        <f t="shared" si="4"/>
+        <v>https://www.schrott-ankauf-wuppertal.de</v>
       </c>
       <c r="B233" s="4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A234" t="str">
-        <f t="shared" si="3"/>
-        <v>https://www.schrottlohmar.de</v>
+        <f t="shared" si="4"/>
+        <v>https://www.schrott-recklinghausen.de</v>
       </c>
       <c r="B234" s="4" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A235" t="str">
-        <f t="shared" si="3"/>
-        <v>https://www.schrottolpe.de</v>
+        <f t="shared" si="4"/>
+        <v>https://www.schrottgummersbach.de</v>
       </c>
       <c r="B235" s="4" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A236" t="str">
-        <f t="shared" si="3"/>
-        <v>https://www.schrottratingen.de</v>
+        <f t="shared" si="4"/>
+        <v>https://www.schrottlohmar.de</v>
       </c>
       <c r="B236" s="4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A237" t="str">
-        <f t="shared" si="3"/>
-        <v>https://www.schrottsiegburg.de</v>
+        <f t="shared" si="4"/>
+        <v>https://www.schrottolpe.de</v>
       </c>
       <c r="B237" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A238" t="str">
-        <f t="shared" si="3"/>
-        <v>https://www.schrottunna.de</v>
+        <f t="shared" si="4"/>
+        <v>https://www.schrottratingen.de</v>
       </c>
       <c r="B238" s="4" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A239" t="str">
-        <f t="shared" si="3"/>
-        <v>https://www.amjis.com</v>
-      </c>
-      <c r="B239" s="5" t="s">
-        <v>229</v>
+        <f t="shared" si="4"/>
+        <v>https://www.schrottsiegburg.de</v>
+      </c>
+      <c r="B239" s="4" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A240" t="str">
-        <f t="shared" si="3"/>
-        <v>https://www.ilamecca.com</v>
-      </c>
-      <c r="B240" s="5" t="s">
-        <v>236</v>
+        <f t="shared" si="4"/>
+        <v>https://www.schrottunna.de</v>
+      </c>
+      <c r="B240" s="4" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A241" t="str">
-        <f t="shared" si="3"/>
-        <v>https://www.kalender.amjis.com</v>
+        <f t="shared" si="4"/>
+        <v>https://www.smarttech-elektro.de</v>
       </c>
       <c r="B241" s="5" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A242" t="str">
-        <f t="shared" si="3"/>
-        <v>https://www.nivontec.de</v>
-      </c>
-      <c r="B242" s="5" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A243" t="str">
-        <f t="shared" si="3"/>
-        <v>https://www.nordstern.gmbh</v>
-      </c>
-      <c r="B243" s="5" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A244" t="str">
-        <f t="shared" si="3"/>
-        <v>https://www.nma-hamburg.de</v>
-      </c>
-      <c r="B244" s="5" t="s">
         <v>233</v>
-      </c>
-    </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A245" t="str">
-        <f t="shared" si="3"/>
-        <v>https://www.smarttech-elektro.de</v>
-      </c>
-      <c r="B245" s="5" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A246" t="str">
-        <f>"https://" &amp; B246</f>
-        <v>https://dr-elrafei.de</v>
-      </c>
-      <c r="B246" t="s">
-        <v>235</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
stonepulse from .de to .com
</commit_message>
<xml_diff>
--- a/src/test/resources/excelData.xlsx
+++ b/src/test/resources/excelData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ibrahim\IdeaProjects\webseit-test\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71943361-3102-4B8E-BF5C-1EDC6279891E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1646C2D9-4E83-4190-937F-5EF7FC969C73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12240" xr2:uid="{1A0E7E13-4B51-4D68-A319-BB2E1A6F5F75}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1A0E7E13-4B51-4D68-A319-BB2E1A6F5F75}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -747,13 +747,13 @@
     <t>https://wiki.nordstern.gmbh/index.php?title=Hauptseite</t>
   </si>
   <si>
-    <t>key.stonepulse.de</t>
-  </si>
-  <si>
-    <t>todo.stonepulse.de</t>
-  </si>
-  <si>
-    <t>kalender.stonepulse.de</t>
+    <t>key.stonepulse.com</t>
+  </si>
+  <si>
+    <t>kalender.stonepulse.com</t>
+  </si>
+  <si>
+    <t>todo.stonepulse.com</t>
   </si>
 </sst>
 </file>
@@ -1150,7 +1150,7 @@
   <dimension ref="A1:B241"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1171,7 +1171,7 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f t="shared" ref="A2:A4" si="0">"https://www." &amp; B2</f>
-        <v>https://www.key.stonepulse.de</v>
+        <v>https://www.key.stonepulse.com</v>
       </c>
       <c r="B2" t="s">
         <v>237</v>
@@ -1180,19 +1180,19 @@
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <f t="shared" si="0"/>
-        <v>https://www.kalender.stonepulse.de</v>
+        <v>https://www.kalender.stonepulse.com</v>
       </c>
       <c r="B3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
-        <v>https://www.todo.stonepulse.de</v>
+        <v>https://www.todo.stonepulse.com</v>
       </c>
       <c r="B4" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>